<commit_message>
wall on xlsx fsile
</commit_message>
<xml_diff>
--- a/hand.xlsx
+++ b/hand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthieu\Documents\Ecole\TelecomSaintEtienne\FISE2\S8\Bibliotheque_de_developpement\hand-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2090B856-E498-4786-8CEE-61509820C0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71501CFA-36BD-457E-B2D7-0157AA35FB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{87BC0737-AAFA-4063-9174-5F881CCA0B83}"/>
   </bookViews>
@@ -35,7 +35,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +96,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -109,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -123,6 +135,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94681083-6FB2-4A7A-A80A-27BF6ABD10B2}">
-  <dimension ref="A1:BB49"/>
+  <dimension ref="A1:BB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AW16" sqref="AW16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="82" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD45" sqref="AD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1106,10 +1120,56 @@
     <row r="26" spans="4:53" x14ac:dyDescent="0.35">
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
+      <c r="AE26" s="12"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="12"/>
+      <c r="AH26" s="12"/>
+      <c r="AI26" s="12"/>
+      <c r="AJ26" s="12"/>
+      <c r="AK26" s="12"/>
+      <c r="AL26" s="12"/>
+      <c r="AM26" s="12"/>
+      <c r="AN26" s="12"/>
+      <c r="AO26" s="12"/>
+      <c r="AP26" s="12"/>
+      <c r="AQ26" s="12"/>
+      <c r="AR26" s="12"/>
+      <c r="AS26" s="12"/>
+      <c r="AT26" s="12"/>
+      <c r="AU26" s="12"/>
     </row>
     <row r="27" spans="4:53" x14ac:dyDescent="0.35">
       <c r="H27" s="1"/>
       <c r="K27" s="1"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="12"/>
+      <c r="AE27" s="12"/>
+      <c r="AF27" s="12"/>
+      <c r="AG27" s="12"/>
+      <c r="AH27" s="12"/>
+      <c r="AI27" s="12"/>
+      <c r="AJ27" s="12"/>
+      <c r="AK27" s="12"/>
+      <c r="AL27" s="12"/>
+      <c r="AM27" s="12"/>
+      <c r="AN27" s="12"/>
+      <c r="AO27" s="12"/>
+      <c r="AP27" s="12"/>
+      <c r="AQ27" s="12"/>
+      <c r="AR27" s="12"/>
+      <c r="AS27" s="12"/>
+      <c r="AT27" s="12"/>
+      <c r="AU27" s="12"/>
     </row>
     <row r="28" spans="4:53" x14ac:dyDescent="0.35">
       <c r="F28" s="1"/>
@@ -1118,6 +1178,29 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="12"/>
+      <c r="AE28" s="12"/>
+      <c r="AF28" s="12"/>
+      <c r="AG28" s="12"/>
+      <c r="AH28" s="12"/>
+      <c r="AI28" s="12"/>
+      <c r="AJ28" s="12"/>
+      <c r="AK28" s="12"/>
+      <c r="AL28" s="12"/>
+      <c r="AM28" s="12"/>
+      <c r="AN28" s="12"/>
+      <c r="AO28" s="12"/>
+      <c r="AP28" s="12"/>
+      <c r="AQ28" s="12"/>
+      <c r="AR28" s="12"/>
+      <c r="AS28" s="12"/>
+      <c r="AT28" s="12"/>
+      <c r="AU28" s="12"/>
     </row>
     <row r="29" spans="4:53" x14ac:dyDescent="0.35">
       <c r="E29" s="1"/>
@@ -1126,6 +1209,29 @@
       <c r="H29" s="1"/>
       <c r="K29" s="1"/>
       <c r="N29" s="1"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="12"/>
+      <c r="AD29" s="12"/>
+      <c r="AE29" s="12"/>
+      <c r="AF29" s="12"/>
+      <c r="AG29" s="12"/>
+      <c r="AH29" s="12"/>
+      <c r="AI29" s="12"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="12"/>
+      <c r="AM29" s="12"/>
+      <c r="AN29" s="12"/>
+      <c r="AO29" s="12"/>
+      <c r="AP29" s="12"/>
+      <c r="AQ29" s="12"/>
+      <c r="AR29" s="12"/>
+      <c r="AS29" s="12"/>
+      <c r="AT29" s="12"/>
+      <c r="AU29" s="12"/>
     </row>
     <row r="30" spans="4:53" x14ac:dyDescent="0.35">
       <c r="E30" s="1"/>
@@ -1134,6 +1240,29 @@
       <c r="H30" s="1"/>
       <c r="K30" s="1"/>
       <c r="N30" s="1"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="12"/>
+      <c r="AD30" s="12"/>
+      <c r="AE30" s="12"/>
+      <c r="AF30" s="12"/>
+      <c r="AG30" s="12"/>
+      <c r="AH30" s="12"/>
+      <c r="AI30" s="1"/>
+      <c r="AJ30" s="11"/>
+      <c r="AK30" s="11"/>
+      <c r="AL30" s="1"/>
+      <c r="AM30" s="12"/>
+      <c r="AN30" s="12"/>
+      <c r="AO30" s="12"/>
+      <c r="AP30" s="12"/>
+      <c r="AQ30" s="12"/>
+      <c r="AR30" s="12"/>
+      <c r="AS30" s="12"/>
+      <c r="AT30" s="12"/>
+      <c r="AU30" s="12"/>
     </row>
     <row r="31" spans="4:53" x14ac:dyDescent="0.35">
       <c r="E31" s="1"/>
@@ -1144,6 +1273,29 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
+      <c r="Y31" s="12"/>
+      <c r="Z31" s="12"/>
+      <c r="AA31" s="12"/>
+      <c r="AB31" s="12"/>
+      <c r="AC31" s="12"/>
+      <c r="AD31" s="12"/>
+      <c r="AE31" s="12"/>
+      <c r="AF31" s="12"/>
+      <c r="AG31" s="1"/>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="11"/>
+      <c r="AK31" s="11"/>
+      <c r="AL31" s="1"/>
+      <c r="AM31" s="1"/>
+      <c r="AN31" s="1"/>
+      <c r="AO31" s="12"/>
+      <c r="AP31" s="12"/>
+      <c r="AQ31" s="12"/>
+      <c r="AR31" s="12"/>
+      <c r="AS31" s="12"/>
+      <c r="AT31" s="12"/>
+      <c r="AU31" s="12"/>
     </row>
     <row r="32" spans="4:53" x14ac:dyDescent="0.35">
       <c r="E32" s="1"/>
@@ -1153,8 +1305,31 @@
       <c r="K32" s="1"/>
       <c r="N32" s="1"/>
       <c r="Q32" s="1"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y32" s="12"/>
+      <c r="Z32" s="12"/>
+      <c r="AA32" s="12"/>
+      <c r="AB32" s="12"/>
+      <c r="AC32" s="12"/>
+      <c r="AD32" s="12"/>
+      <c r="AE32" s="12"/>
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="11"/>
+      <c r="AH32" s="11"/>
+      <c r="AI32" s="1"/>
+      <c r="AJ32" s="11"/>
+      <c r="AK32" s="11"/>
+      <c r="AL32" s="1"/>
+      <c r="AM32" s="11"/>
+      <c r="AN32" s="11"/>
+      <c r="AO32" s="1"/>
+      <c r="AP32" s="12"/>
+      <c r="AQ32" s="12"/>
+      <c r="AR32" s="12"/>
+      <c r="AS32" s="12"/>
+      <c r="AT32" s="12"/>
+      <c r="AU32" s="12"/>
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="E33" s="1"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -1164,8 +1339,31 @@
       <c r="K33" s="10"/>
       <c r="N33" s="1"/>
       <c r="Q33" s="1"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y33" s="12"/>
+      <c r="Z33" s="12"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="12"/>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="12"/>
+      <c r="AF33" s="1"/>
+      <c r="AG33" s="11"/>
+      <c r="AH33" s="11"/>
+      <c r="AI33" s="1"/>
+      <c r="AJ33" s="11"/>
+      <c r="AK33" s="11"/>
+      <c r="AL33" s="1"/>
+      <c r="AM33" s="11"/>
+      <c r="AN33" s="11"/>
+      <c r="AO33" s="1"/>
+      <c r="AP33" s="12"/>
+      <c r="AQ33" s="12"/>
+      <c r="AR33" s="12"/>
+      <c r="AS33" s="12"/>
+      <c r="AT33" s="12"/>
+      <c r="AU33" s="12"/>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="E34" s="10"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
@@ -1177,8 +1375,31 @@
       <c r="M34" s="8"/>
       <c r="N34" s="10"/>
       <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y34" s="12"/>
+      <c r="Z34" s="12"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="12"/>
+      <c r="AD34" s="12"/>
+      <c r="AE34" s="12"/>
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="11"/>
+      <c r="AH34" s="11"/>
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="11"/>
+      <c r="AK34" s="11"/>
+      <c r="AL34" s="1"/>
+      <c r="AM34" s="11"/>
+      <c r="AN34" s="11"/>
+      <c r="AO34" s="1"/>
+      <c r="AP34" s="1"/>
+      <c r="AQ34" s="1"/>
+      <c r="AR34" s="12"/>
+      <c r="AS34" s="12"/>
+      <c r="AT34" s="12"/>
+      <c r="AU34" s="12"/>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="E35" s="10"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
@@ -1191,8 +1412,31 @@
       <c r="N35" s="10"/>
       <c r="O35" s="8"/>
       <c r="Q35" s="10"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y35" s="12"/>
+      <c r="Z35" s="12"/>
+      <c r="AA35" s="12"/>
+      <c r="AB35" s="12"/>
+      <c r="AC35" s="12"/>
+      <c r="AD35" s="12"/>
+      <c r="AE35" s="12"/>
+      <c r="AF35" s="1"/>
+      <c r="AG35" s="11"/>
+      <c r="AH35" s="11"/>
+      <c r="AI35" s="1"/>
+      <c r="AJ35" s="11"/>
+      <c r="AK35" s="11"/>
+      <c r="AL35" s="1"/>
+      <c r="AM35" s="11"/>
+      <c r="AN35" s="11"/>
+      <c r="AO35" s="1"/>
+      <c r="AP35" s="11"/>
+      <c r="AQ35" s="11"/>
+      <c r="AR35" s="1"/>
+      <c r="AS35" s="12"/>
+      <c r="AT35" s="12"/>
+      <c r="AU35" s="12"/>
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="E36" s="10"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
@@ -1206,8 +1450,31 @@
       <c r="O36" s="8"/>
       <c r="P36" s="8"/>
       <c r="Q36" s="10"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y36" s="12"/>
+      <c r="Z36" s="12"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="12"/>
+      <c r="AC36" s="12"/>
+      <c r="AD36" s="12"/>
+      <c r="AE36" s="12"/>
+      <c r="AF36" s="1"/>
+      <c r="AG36" s="11"/>
+      <c r="AH36" s="11"/>
+      <c r="AI36" s="1"/>
+      <c r="AJ36" s="11"/>
+      <c r="AK36" s="11"/>
+      <c r="AL36" s="1"/>
+      <c r="AM36" s="11"/>
+      <c r="AN36" s="11"/>
+      <c r="AO36" s="1"/>
+      <c r="AP36" s="11"/>
+      <c r="AQ36" s="11"/>
+      <c r="AR36" s="1"/>
+      <c r="AS36" s="12"/>
+      <c r="AT36" s="12"/>
+      <c r="AU36" s="12"/>
+    </row>
+    <row r="37" spans="1:47" x14ac:dyDescent="0.35">
       <c r="E37" s="10"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -1221,8 +1488,31 @@
       <c r="O37" s="8"/>
       <c r="P37" s="8"/>
       <c r="Q37" s="10"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y37" s="12"/>
+      <c r="Z37" s="12"/>
+      <c r="AA37" s="12"/>
+      <c r="AB37" s="12"/>
+      <c r="AC37" s="12"/>
+      <c r="AD37" s="12"/>
+      <c r="AE37" s="12"/>
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="11"/>
+      <c r="AH37" s="11"/>
+      <c r="AI37" s="1"/>
+      <c r="AJ37" s="11"/>
+      <c r="AK37" s="11"/>
+      <c r="AL37" s="1"/>
+      <c r="AM37" s="11"/>
+      <c r="AN37" s="11"/>
+      <c r="AO37" s="1"/>
+      <c r="AP37" s="11"/>
+      <c r="AQ37" s="11"/>
+      <c r="AR37" s="1"/>
+      <c r="AS37" s="12"/>
+      <c r="AT37" s="12"/>
+      <c r="AU37" s="12"/>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1239,8 +1529,31 @@
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
       <c r="Q38" s="10"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y38" s="12"/>
+      <c r="Z38" s="12"/>
+      <c r="AA38" s="12"/>
+      <c r="AB38" s="12"/>
+      <c r="AC38" s="12"/>
+      <c r="AD38" s="12"/>
+      <c r="AE38" s="12"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="11"/>
+      <c r="AH38" s="11"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="11"/>
+      <c r="AK38" s="11"/>
+      <c r="AL38" s="1"/>
+      <c r="AM38" s="11"/>
+      <c r="AN38" s="11"/>
+      <c r="AO38" s="1"/>
+      <c r="AP38" s="11"/>
+      <c r="AQ38" s="11"/>
+      <c r="AR38" s="1"/>
+      <c r="AS38" s="12"/>
+      <c r="AT38" s="12"/>
+      <c r="AU38" s="12"/>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -1256,8 +1569,31 @@
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
       <c r="Q39" s="10"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y39" s="12"/>
+      <c r="Z39" s="12"/>
+      <c r="AA39" s="12"/>
+      <c r="AB39" s="12"/>
+      <c r="AC39" s="12"/>
+      <c r="AD39" s="12"/>
+      <c r="AE39" s="12"/>
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="11"/>
+      <c r="AH39" s="11"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="11"/>
+      <c r="AK39" s="11"/>
+      <c r="AL39" s="1"/>
+      <c r="AM39" s="11"/>
+      <c r="AN39" s="11"/>
+      <c r="AO39" s="1"/>
+      <c r="AP39" s="11"/>
+      <c r="AQ39" s="11"/>
+      <c r="AR39" s="1"/>
+      <c r="AS39" s="12"/>
+      <c r="AT39" s="12"/>
+      <c r="AU39" s="12"/>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="D40" s="8"/>
       <c r="E40" s="10"/>
@@ -1273,8 +1609,31 @@
       <c r="O40" s="8"/>
       <c r="P40" s="8"/>
       <c r="Q40" s="10"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y40" s="12"/>
+      <c r="Z40" s="12"/>
+      <c r="AA40" s="12"/>
+      <c r="AB40" s="12"/>
+      <c r="AC40" s="12"/>
+      <c r="AD40" s="12"/>
+      <c r="AE40" s="12"/>
+      <c r="AF40" s="1"/>
+      <c r="AG40" s="11"/>
+      <c r="AH40" s="11"/>
+      <c r="AI40" s="1"/>
+      <c r="AJ40" s="11"/>
+      <c r="AK40" s="11"/>
+      <c r="AL40" s="1"/>
+      <c r="AM40" s="11"/>
+      <c r="AN40" s="11"/>
+      <c r="AO40" s="1"/>
+      <c r="AP40" s="11"/>
+      <c r="AQ40" s="11"/>
+      <c r="AR40" s="1"/>
+      <c r="AS40" s="12"/>
+      <c r="AT40" s="12"/>
+      <c r="AU40" s="12"/>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.35">
       <c r="B41" s="1"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -1291,8 +1650,31 @@
       <c r="O41" s="8"/>
       <c r="P41" s="8"/>
       <c r="Q41" s="10"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y41" s="12"/>
+      <c r="Z41" s="12"/>
+      <c r="AA41" s="12"/>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="12"/>
+      <c r="AF41" s="1"/>
+      <c r="AG41" s="11"/>
+      <c r="AH41" s="11"/>
+      <c r="AI41" s="11"/>
+      <c r="AJ41" s="11"/>
+      <c r="AK41" s="11"/>
+      <c r="AL41" s="11"/>
+      <c r="AM41" s="11"/>
+      <c r="AN41" s="11"/>
+      <c r="AO41" s="11"/>
+      <c r="AP41" s="11"/>
+      <c r="AQ41" s="11"/>
+      <c r="AR41" s="1"/>
+      <c r="AS41" s="12"/>
+      <c r="AT41" s="12"/>
+      <c r="AU41" s="12"/>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.35">
       <c r="C42" s="1"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -1308,8 +1690,31 @@
       <c r="O42" s="8"/>
       <c r="P42" s="8"/>
       <c r="Q42" s="10"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y42" s="12"/>
+      <c r="Z42" s="12"/>
+      <c r="AA42" s="12"/>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="11"/>
+      <c r="AD42" s="11"/>
+      <c r="AE42" s="1"/>
+      <c r="AF42" s="1"/>
+      <c r="AG42" s="11"/>
+      <c r="AH42" s="11"/>
+      <c r="AI42" s="11"/>
+      <c r="AJ42" s="11"/>
+      <c r="AK42" s="11"/>
+      <c r="AL42" s="11"/>
+      <c r="AM42" s="11"/>
+      <c r="AN42" s="11"/>
+      <c r="AO42" s="11"/>
+      <c r="AP42" s="11"/>
+      <c r="AQ42" s="11"/>
+      <c r="AR42" s="1"/>
+      <c r="AS42" s="12"/>
+      <c r="AT42" s="12"/>
+      <c r="AU42" s="12"/>
+    </row>
+    <row r="43" spans="1:47" x14ac:dyDescent="0.35">
       <c r="C43" s="10"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -1325,8 +1730,31 @@
       <c r="O43" s="8"/>
       <c r="P43" s="8"/>
       <c r="Q43" s="10"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y43" s="12"/>
+      <c r="Z43" s="12"/>
+      <c r="AA43" s="12"/>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="11"/>
+      <c r="AD43" s="11"/>
+      <c r="AE43" s="11"/>
+      <c r="AF43" s="1"/>
+      <c r="AG43" s="11"/>
+      <c r="AH43" s="11"/>
+      <c r="AI43" s="11"/>
+      <c r="AJ43" s="11"/>
+      <c r="AK43" s="11"/>
+      <c r="AL43" s="11"/>
+      <c r="AM43" s="11"/>
+      <c r="AN43" s="11"/>
+      <c r="AO43" s="11"/>
+      <c r="AP43" s="11"/>
+      <c r="AQ43" s="11"/>
+      <c r="AR43" s="1"/>
+      <c r="AS43" s="12"/>
+      <c r="AT43" s="12"/>
+      <c r="AU43" s="12"/>
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.35">
       <c r="D44" s="10"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -1340,8 +1768,31 @@
       <c r="N44" s="8"/>
       <c r="O44" s="8"/>
       <c r="P44" s="10"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y44" s="12"/>
+      <c r="Z44" s="12"/>
+      <c r="AA44" s="12"/>
+      <c r="AB44" s="12"/>
+      <c r="AC44" s="1"/>
+      <c r="AD44" s="11"/>
+      <c r="AE44" s="11"/>
+      <c r="AF44" s="1"/>
+      <c r="AG44" s="11"/>
+      <c r="AH44" s="11"/>
+      <c r="AI44" s="11"/>
+      <c r="AJ44" s="11"/>
+      <c r="AK44" s="3"/>
+      <c r="AL44" s="11"/>
+      <c r="AM44" s="11"/>
+      <c r="AN44" s="11"/>
+      <c r="AO44" s="11"/>
+      <c r="AP44" s="11"/>
+      <c r="AQ44" s="11"/>
+      <c r="AR44" s="1"/>
+      <c r="AS44" s="12"/>
+      <c r="AT44" s="12"/>
+      <c r="AU44" s="12"/>
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.35">
       <c r="D45" s="10"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
@@ -1355,8 +1806,31 @@
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
       <c r="P45" s="10"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="12"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="12"/>
+      <c r="AC45" s="12"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="11"/>
+      <c r="AF45" s="11"/>
+      <c r="AG45" s="11"/>
+      <c r="AH45" s="11"/>
+      <c r="AI45" s="11"/>
+      <c r="AJ45" s="11"/>
+      <c r="AK45" s="11"/>
+      <c r="AL45" s="11"/>
+      <c r="AM45" s="11"/>
+      <c r="AN45" s="11"/>
+      <c r="AO45" s="11"/>
+      <c r="AP45" s="11"/>
+      <c r="AQ45" s="11"/>
+      <c r="AR45" s="1"/>
+      <c r="AS45" s="12"/>
+      <c r="AT45" s="12"/>
+      <c r="AU45" s="12"/>
+    </row>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.35">
       <c r="E46" s="10"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -1368,8 +1842,31 @@
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
       <c r="O46" s="10"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y46" s="12"/>
+      <c r="Z46" s="12"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="12"/>
+      <c r="AC46" s="12"/>
+      <c r="AD46" s="1"/>
+      <c r="AE46" s="11"/>
+      <c r="AF46" s="11"/>
+      <c r="AG46" s="11"/>
+      <c r="AH46" s="11"/>
+      <c r="AI46" s="11"/>
+      <c r="AJ46" s="11"/>
+      <c r="AK46" s="11"/>
+      <c r="AL46" s="11"/>
+      <c r="AM46" s="11"/>
+      <c r="AN46" s="11"/>
+      <c r="AO46" s="11"/>
+      <c r="AP46" s="11"/>
+      <c r="AQ46" s="11"/>
+      <c r="AR46" s="1"/>
+      <c r="AS46" s="12"/>
+      <c r="AT46" s="12"/>
+      <c r="AU46" s="12"/>
+    </row>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.35">
       <c r="E47" s="10"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
@@ -1381,8 +1878,31 @@
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
       <c r="O47" s="10"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Y47" s="12"/>
+      <c r="Z47" s="12"/>
+      <c r="AA47" s="12"/>
+      <c r="AB47" s="12"/>
+      <c r="AC47" s="12"/>
+      <c r="AD47" s="12"/>
+      <c r="AE47" s="1"/>
+      <c r="AF47" s="11"/>
+      <c r="AG47" s="11"/>
+      <c r="AH47" s="11"/>
+      <c r="AI47" s="11"/>
+      <c r="AJ47" s="11"/>
+      <c r="AK47" s="11"/>
+      <c r="AL47" s="11"/>
+      <c r="AM47" s="11"/>
+      <c r="AN47" s="11"/>
+      <c r="AO47" s="11"/>
+      <c r="AP47" s="11"/>
+      <c r="AQ47" s="1"/>
+      <c r="AR47" s="12"/>
+      <c r="AS47" s="12"/>
+      <c r="AT47" s="12"/>
+      <c r="AU47" s="12"/>
+    </row>
+    <row r="48" spans="1:47" x14ac:dyDescent="0.35">
       <c r="F48" s="10"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
@@ -1393,8 +1913,31 @@
       <c r="M48" s="8"/>
       <c r="N48" s="8"/>
       <c r="O48" s="10"/>
-    </row>
-    <row r="49" spans="6:15" x14ac:dyDescent="0.35">
+      <c r="Y48" s="12"/>
+      <c r="Z48" s="12"/>
+      <c r="AA48" s="12"/>
+      <c r="AB48" s="12"/>
+      <c r="AC48" s="12"/>
+      <c r="AD48" s="12"/>
+      <c r="AE48" s="1"/>
+      <c r="AF48" s="11"/>
+      <c r="AG48" s="11"/>
+      <c r="AH48" s="11"/>
+      <c r="AI48" s="11"/>
+      <c r="AJ48" s="11"/>
+      <c r="AK48" s="11"/>
+      <c r="AL48" s="11"/>
+      <c r="AM48" s="11"/>
+      <c r="AN48" s="11"/>
+      <c r="AO48" s="11"/>
+      <c r="AP48" s="11"/>
+      <c r="AQ48" s="1"/>
+      <c r="AR48" s="12"/>
+      <c r="AS48" s="12"/>
+      <c r="AT48" s="12"/>
+      <c r="AU48" s="12"/>
+    </row>
+    <row r="49" spans="6:47" x14ac:dyDescent="0.35">
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
@@ -1405,6 +1948,179 @@
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
+      <c r="Y49" s="12"/>
+      <c r="Z49" s="12"/>
+      <c r="AA49" s="12"/>
+      <c r="AB49" s="12"/>
+      <c r="AC49" s="12"/>
+      <c r="AD49" s="12"/>
+      <c r="AE49" s="12"/>
+      <c r="AF49" s="1"/>
+      <c r="AG49" s="11"/>
+      <c r="AH49" s="11"/>
+      <c r="AI49" s="11"/>
+      <c r="AJ49" s="11"/>
+      <c r="AK49" s="11"/>
+      <c r="AL49" s="11"/>
+      <c r="AM49" s="11"/>
+      <c r="AN49" s="11"/>
+      <c r="AO49" s="11"/>
+      <c r="AP49" s="1"/>
+      <c r="AQ49" s="12"/>
+      <c r="AR49" s="12"/>
+      <c r="AS49" s="12"/>
+      <c r="AT49" s="12"/>
+      <c r="AU49" s="12"/>
+    </row>
+    <row r="50" spans="6:47" x14ac:dyDescent="0.35">
+      <c r="Y50" s="12"/>
+      <c r="Z50" s="12"/>
+      <c r="AA50" s="12"/>
+      <c r="AB50" s="12"/>
+      <c r="AC50" s="12"/>
+      <c r="AD50" s="12"/>
+      <c r="AE50" s="12"/>
+      <c r="AF50" s="1"/>
+      <c r="AG50" s="11"/>
+      <c r="AH50" s="11"/>
+      <c r="AI50" s="11"/>
+      <c r="AJ50" s="11"/>
+      <c r="AK50" s="11"/>
+      <c r="AL50" s="11"/>
+      <c r="AM50" s="11"/>
+      <c r="AN50" s="11"/>
+      <c r="AO50" s="11"/>
+      <c r="AP50" s="1"/>
+      <c r="AQ50" s="12"/>
+      <c r="AR50" s="12"/>
+      <c r="AS50" s="12"/>
+      <c r="AT50" s="12"/>
+      <c r="AU50" s="12"/>
+    </row>
+    <row r="51" spans="6:47" x14ac:dyDescent="0.35">
+      <c r="Y51" s="12"/>
+      <c r="Z51" s="12"/>
+      <c r="AA51" s="12"/>
+      <c r="AB51" s="12"/>
+      <c r="AC51" s="12"/>
+      <c r="AD51" s="12"/>
+      <c r="AE51" s="12"/>
+      <c r="AF51" s="12"/>
+      <c r="AG51" s="1"/>
+      <c r="AH51" s="11"/>
+      <c r="AI51" s="11"/>
+      <c r="AJ51" s="11"/>
+      <c r="AK51" s="11"/>
+      <c r="AL51" s="11"/>
+      <c r="AM51" s="11"/>
+      <c r="AN51" s="11"/>
+      <c r="AO51" s="11"/>
+      <c r="AP51" s="1"/>
+      <c r="AQ51" s="12"/>
+      <c r="AR51" s="12"/>
+      <c r="AS51" s="12"/>
+      <c r="AT51" s="12"/>
+      <c r="AU51" s="12"/>
+    </row>
+    <row r="52" spans="6:47" x14ac:dyDescent="0.35">
+      <c r="Y52" s="12"/>
+      <c r="Z52" s="12"/>
+      <c r="AA52" s="12"/>
+      <c r="AB52" s="12"/>
+      <c r="AC52" s="12"/>
+      <c r="AD52" s="12"/>
+      <c r="AE52" s="12"/>
+      <c r="AF52" s="12"/>
+      <c r="AG52" s="1"/>
+      <c r="AH52" s="1"/>
+      <c r="AI52" s="1"/>
+      <c r="AJ52" s="1"/>
+      <c r="AK52" s="1"/>
+      <c r="AL52" s="1"/>
+      <c r="AM52" s="1"/>
+      <c r="AN52" s="1"/>
+      <c r="AO52" s="1"/>
+      <c r="AP52" s="1"/>
+      <c r="AQ52" s="12"/>
+      <c r="AR52" s="12"/>
+      <c r="AS52" s="12"/>
+      <c r="AT52" s="12"/>
+      <c r="AU52" s="12"/>
+    </row>
+    <row r="53" spans="6:47" x14ac:dyDescent="0.35">
+      <c r="Y53" s="12"/>
+      <c r="Z53" s="12"/>
+      <c r="AA53" s="12"/>
+      <c r="AB53" s="12"/>
+      <c r="AC53" s="12"/>
+      <c r="AD53" s="12"/>
+      <c r="AE53" s="12"/>
+      <c r="AF53" s="12"/>
+      <c r="AG53" s="12"/>
+      <c r="AH53" s="12"/>
+      <c r="AI53" s="12"/>
+      <c r="AJ53" s="12"/>
+      <c r="AK53" s="12"/>
+      <c r="AL53" s="12"/>
+      <c r="AM53" s="12"/>
+      <c r="AN53" s="12"/>
+      <c r="AO53" s="12"/>
+      <c r="AP53" s="12"/>
+      <c r="AQ53" s="12"/>
+      <c r="AR53" s="12"/>
+      <c r="AS53" s="12"/>
+      <c r="AT53" s="12"/>
+      <c r="AU53" s="12"/>
+    </row>
+    <row r="54" spans="6:47" x14ac:dyDescent="0.35">
+      <c r="Y54" s="12"/>
+      <c r="Z54" s="12"/>
+      <c r="AA54" s="12"/>
+      <c r="AB54" s="12"/>
+      <c r="AC54" s="12"/>
+      <c r="AD54" s="12"/>
+      <c r="AE54" s="12"/>
+      <c r="AF54" s="12"/>
+      <c r="AG54" s="12"/>
+      <c r="AH54" s="12"/>
+      <c r="AI54" s="12"/>
+      <c r="AJ54" s="12"/>
+      <c r="AK54" s="12"/>
+      <c r="AL54" s="12"/>
+      <c r="AM54" s="12"/>
+      <c r="AN54" s="12"/>
+      <c r="AO54" s="12"/>
+      <c r="AP54" s="12"/>
+      <c r="AQ54" s="12"/>
+      <c r="AR54" s="12"/>
+      <c r="AS54" s="12"/>
+      <c r="AT54" s="12"/>
+      <c r="AU54" s="12"/>
+    </row>
+    <row r="55" spans="6:47" x14ac:dyDescent="0.35">
+      <c r="Y55" s="12"/>
+      <c r="Z55" s="12"/>
+      <c r="AA55" s="12"/>
+      <c r="AB55" s="12"/>
+      <c r="AC55" s="12"/>
+      <c r="AD55" s="12"/>
+      <c r="AE55" s="12"/>
+      <c r="AF55" s="12"/>
+      <c r="AG55" s="12"/>
+      <c r="AH55" s="12"/>
+      <c r="AI55" s="12"/>
+      <c r="AJ55" s="12"/>
+      <c r="AK55" s="12"/>
+      <c r="AL55" s="12"/>
+      <c r="AM55" s="12"/>
+      <c r="AN55" s="12"/>
+      <c r="AO55" s="12"/>
+      <c r="AP55" s="12"/>
+      <c r="AQ55" s="12"/>
+      <c r="AR55" s="12"/>
+      <c r="AS55" s="12"/>
+      <c r="AT55" s="12"/>
+      <c r="AU55" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>